<commit_message>
classwork i and ii done
</commit_message>
<xml_diff>
--- a/my-mini-corpus-bogazici-university.xlsx
+++ b/my-mini-corpus-bogazici-university.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\özgür deniz\Desktop\my-mini-corpus-bogazici-university\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DD6C77-725A-40F4-AE08-89A25C2C5D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23000025-D457-46CF-911A-15F43E11416E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sources" sheetId="1" r:id="rId1"/>
+    <sheet name="WordFreqList" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Source</t>
   </si>
@@ -136,6 +137,54 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ve</t>
+  </si>
+  <si>
+    <t>bir</t>
+  </si>
+  <si>
+    <t>bu</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>için</t>
+  </si>
+  <si>
+    <t>ile</t>
+  </si>
+  <si>
+    <t>çok</t>
+  </si>
+  <si>
+    <t>olarak</t>
+  </si>
+  <si>
+    <t>daha</t>
+  </si>
+  <si>
+    <t>TSCorpus</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+  <si>
+    <t>my-mini-corpus</t>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>boğaziçi</t>
   </si>
 </sst>
 </file>
@@ -177,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -195,6 +244,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -692,4 +744,204 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C413A16D-4853-4789-A532-3B8FBF700D1D}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2">
+        <v>8910007</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3">
+        <v>8185200</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>5055490</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>2943937</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>2776962</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>2524628</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <v>1936336</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9">
+        <v>1870108</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>1520288</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11">
+        <v>1440179</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A11"/>
+    <mergeCell ref="E1:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>